<commit_message>
Added new fetures and fixed bugs
</commit_message>
<xml_diff>
--- a/auction_results.xlsx
+++ b/auction_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,44 +462,44 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sandeep</t>
+          <t>Anirudh</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>All Rounder</t>
+          <t>O</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Hritik</t>
+          <t>UNSOLD</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Devesh</t>
+          <t xml:space="preserve">Shubham Panchal </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>All Rounder</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Mangesh</t>
+          <t>DC</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -508,48 +508,136 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Dhananjay (Bachhu)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>DC</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>All Rounder</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>UNSOLD</t>
-        </is>
-      </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mangesh</t>
+          <t xml:space="preserve">Vishal Sawant </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>All Rounder</t>
+          <t>=</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sandeep</t>
+          <t>MI</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>60</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Viraj Ambre</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>UNSOLD</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>34</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ganesh Pandian </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Monish Rathod</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>MI</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>57</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Chetan Shrivastav</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>